<commit_message>
updates on streamlit app
</commit_message>
<xml_diff>
--- a/model_results/auc.xlsx
+++ b/model_results/auc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://allianzms-my.sharepoint.com/personal/falk_kegler_allianz_de/Documents/Sorbonne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34FEE6EE-9AD3-4E35-970A-8230CFDFBF4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{34FEE6EE-9AD3-4E35-970A-8230CFDFBF4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B766708-E200-49B1-B1A3-1176B5E02281}"/>
   <bookViews>
-    <workbookView xWindow="7020" yWindow="0" windowWidth="21360" windowHeight="14805" xr2:uid="{FF4FDE16-A746-4E04-B796-59CF173111B9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28620" windowHeight="15045" xr2:uid="{FF4FDE16-A746-4E04-B796-59CF173111B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Random Forest</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Model</t>
+  </si>
+  <si>
+    <t>K-Nearest Neighbors (k=3)</t>
   </si>
 </sst>
 </file>
@@ -213,37 +216,98 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="bg1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$A$2:$A$4</c:f>
+              <c:f>Tabelle1!$A$2:$A$5</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>XGBoost</c:v>
+                  <c:v>K-Nearest Neighbors (k=3)</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>Random Forest</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>Dense Neural Network</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>Random Forest</c:v>
+                <c:pt idx="3">
+                  <c:v>XGBoost</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$2:$B$4</c:f>
+              <c:f>Tabelle1!$B$2:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.79300000000000004</c:v>
+                <c:ptCount val="4"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0.68799999999999994</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.78700000000000003</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.78</c:v>
+                <c:pt idx="3">
+                  <c:v>0.79300000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -321,6 +385,8 @@
         <c:axId val="782884952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="0.8"/>
+          <c:min val="0.60000000000000009"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -338,7 +404,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -372,6 +438,7 @@
         <c:crossAx val="782887112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="5.000000000000001E-2"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1301,10 +1368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{727C30AC-0A58-4D98-AC13-04539459F5CC}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1322,29 +1389,40 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
-      <c r="B2" s="1">
-        <v>0.79300000000000004</v>
+      <c r="B2">
+        <v>0.68799999999999994</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3" s="1">
-        <v>0.78700000000000003</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>0.78</v>
+        <v>0.78700000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.79300000000000004</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B5">
+    <sortCondition ref="B2:B5"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>